<commit_message>
Nearly complete command parsing
</commit_message>
<xml_diff>
--- a/Java/API Builder/test/test.xlsx
+++ b/Java/API Builder/test/test.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="18195" windowHeight="9015"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,70 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
-  <si>
-    <r>
-      <t xml:space="preserve">Prefix: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>MIT2000</t>
-    </r>
-  </si>
-  <si>
-    <t>]</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">technology: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LabVIEW</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Manufacturer: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>David</t>
-    </r>
-  </si>
-  <si>
-    <t>[Test</t>
-  </si>
-  <si>
-    <t>[test1]</t>
-  </si>
-  <si>
-    <t>[test2]</t>
-  </si>
-  <si>
-    <t>[Analog]</t>
-  </si>
-  <si>
-    <t>[Digital]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <r>
       <rPr>
@@ -90,7 +27,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Identifier:</t>
+      <t>Prefix</t>
     </r>
     <r>
       <rPr>
@@ -100,13 +37,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> My Instrument Test</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
+      <t>: MIT2000</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -116,13 +50,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Configure</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
+      <t>Identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: My Instrument Test</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -132,7 +73,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Action-Status</t>
+      <t>technology</t>
     </r>
     <r>
       <rPr>
@@ -142,13 +83,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
+      <t>: LabVIEW</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -158,15 +96,143 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Manufacturer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: David</t>
+    </r>
+  </si>
+  <si>
+    <t>Configure Frequency</t>
+  </si>
+  <si>
+    <t>Configure Amplitude</t>
+  </si>
+  <si>
+    <t>#This is digital</t>
+  </si>
+  <si>
+    <t>Configure dBM</t>
+  </si>
+  <si>
+    <t>Configure Resolution</t>
+  </si>
+  <si>
+    <t>Read Measurement</t>
+  </si>
+  <si>
+    <t>Read Frequency</t>
+  </si>
+  <si>
+    <t>Read Last Data</t>
+  </si>
+  <si>
+    <t>Read Amplitude</t>
+  </si>
+  <si>
+    <t>{Analog</t>
+  </si>
+  <si>
+    <t>{Digital</t>
+  </si>
+  <si>
+    <t>{Measurements</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>{Quick Measurements}</t>
+  </si>
+  <si>
+    <r>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Configure</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Action-Status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Data</t>
     </r>
+  </si>
+  <si>
+    <t>in:Frequency:double</t>
+  </si>
+  <si>
+    <t>MIT:TEST:FREQ &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>MIT:TEST:AMP &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>in:Amplitude:double</t>
+  </si>
+  <si>
+    <t># Sets the frequency of the analog measurement.</t>
+  </si>
+  <si>
+    <t># Sets the amplitude of the analog measurement.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +243,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -205,7 +286,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,92 +581,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" customWidth="1"/>
+    <col min="6" max="6" width="57.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18.75">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="18.75">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="C25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="26" spans="1:3">
+      <c r="C26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+    <row r="27" spans="1:3">
+      <c r="C27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+    <row r="28" spans="1:3">
+      <c r="C28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>1</v>
+    <row r="29" spans="1:3">
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -598,7 +750,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
Fixed bugs and added corner cases
</commit_message>
<xml_diff>
--- a/Java/API Builder/test/test.xlsx
+++ b/Java/API Builder/test/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <r>
       <rPr>
@@ -210,22 +210,87 @@
     </r>
   </si>
   <si>
-    <t>in:Frequency:double</t>
-  </si>
-  <si>
-    <t>MIT:TEST:FREQ &lt;value&gt;</t>
-  </si>
-  <si>
     <t>MIT:TEST:AMP &lt;value&gt;</t>
   </si>
   <si>
     <t>in:Amplitude:double</t>
   </si>
   <si>
-    <t># Sets the frequency of the analog measurement.</t>
-  </si>
-  <si>
-    <t># Sets the amplitude of the analog measurement.</t>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Utility</t>
+    </r>
+  </si>
+  <si>
+    <t>*RST</t>
+  </si>
+  <si>
+    <t>This is a comment</t>
+  </si>
+  <si>
+    <t>in:dBM:integer</t>
+  </si>
+  <si>
+    <t>MIT:TEST:DBM &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>in:Resoluttion:Double</t>
+  </si>
+  <si>
+    <t>MIT:TEST:RESO &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>#This is analog</t>
+  </si>
+  <si>
+    <t>out:Measurement:Ring:val1,val2,</t>
+  </si>
+  <si>
+    <t>in: Frequency:double</t>
+  </si>
+  <si>
+    <t>out:Frequency:int</t>
+  </si>
+  <si>
+    <t>out:Last Data:string</t>
+  </si>
+  <si>
+    <t>{Configure</t>
+  </si>
+  <si>
+    <t>Im a Vi</t>
+  </si>
+  <si>
+    <t>Sets the amplitude of the analog measurement.</t>
+  </si>
+  <si>
+    <t>#This is a comment</t>
+  </si>
+  <si>
+    <t>{configure</t>
   </si>
 </sst>
 </file>
@@ -581,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -617,6 +682,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="8" spans="1:6" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>18</v>
@@ -627,18 +697,20 @@
         <v>13</v>
       </c>
     </row>
+    <row r="10" spans="1:6">
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="11" spans="1:6">
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -646,13 +718,13 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -674,69 +746,114 @@
       <c r="C16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="C17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="B18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18.75">
+    <row r="21" spans="1:5" ht="18.75">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="18.75">
+    <row r="23" spans="1:5" ht="18.75">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:5">
       <c r="B24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:5">
       <c r="C25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="C26" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="C27" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="C28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="B29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:5">
       <c r="B30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="18.75">
+      <c r="A33" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
         <v>16</v>
       </c>
     </row>
@@ -748,14 +865,64 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D24"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="45" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
OMG IT WORKS, No Vis though
</commit_message>
<xml_diff>
--- a/Java/API Builder/test/test.xlsx
+++ b/Java/API Builder/test/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <r>
       <rPr>
@@ -275,19 +275,48 @@
     <t>out:Last Data:string</t>
   </si>
   <si>
-    <t>{Configure</t>
-  </si>
-  <si>
-    <t>Im a Vi</t>
-  </si>
-  <si>
-    <t>Sets the amplitude of the analog measurement.</t>
-  </si>
-  <si>
     <t>#This is a comment</t>
   </si>
   <si>
-    <t>{configure</t>
+    <t>#Sets the amplitude of the analog measurement.</t>
+  </si>
+  <si>
+    <t>{Analog}</t>
+  </si>
+  <si>
+    <t>{Action-Status}</t>
+  </si>
+  <si>
+    <t>Configure Digital Frequency</t>
+  </si>
+  <si>
+    <t>MIT:DIG:FREQ &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>abc:Frequency:double</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>technology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: LabVIEW PNP</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -346,9 +375,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -671,7 +701,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -707,7 +737,7 @@
         <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -721,7 +751,7 @@
         <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -862,61 +892,77 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:B11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="45" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    <row r="6" spans="1:5" ht="18.75">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>40</v>
+    <row r="10" spans="1:5">
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18.75">
+      <c r="A13" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented multi-control Vis, started write out for Vis and controls
</commit_message>
<xml_diff>
--- a/Java/API Builder/test/test.xlsx
+++ b/Java/API Builder/test/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="18195" windowHeight="9015"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="18195" windowHeight="9015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <r>
       <rPr>
@@ -281,42 +281,58 @@
     <t>#Sets the amplitude of the analog measurement.</t>
   </si>
   <si>
-    <t>{Analog}</t>
-  </si>
-  <si>
-    <t>{Action-Status}</t>
-  </si>
-  <si>
-    <t>Configure Digital Frequency</t>
-  </si>
-  <si>
-    <t>MIT:DIG:FREQ &lt;value&gt;</t>
-  </si>
-  <si>
-    <t>abc:Frequency:double</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>technology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: LabVIEW PNP</t>
-    </r>
+    <t>{how</t>
+  </si>
+  <si>
+    <t>{far</t>
+  </si>
+  <si>
+    <t>{down</t>
+  </si>
+  <si>
+    <t>{can</t>
+  </si>
+  <si>
+    <t>{this</t>
+  </si>
+  <si>
+    <t>{will</t>
+  </si>
+  <si>
+    <t>{go?}</t>
+  </si>
+  <si>
+    <t>My Vi</t>
+  </si>
+  <si>
+    <t>in:Test2:double</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>MIT:TEST:TEST1 &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>MIT:TEST:TEST2 &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>Vi2</t>
+  </si>
+  <si>
+    <t>in:Test3:double</t>
+  </si>
+  <si>
+    <t>in:Test4:double</t>
+  </si>
+  <si>
+    <t>{utility</t>
+  </si>
+  <si>
+    <t>{lower}</t>
+  </si>
+  <si>
+    <t>in:Test1:integer</t>
   </si>
 </sst>
 </file>
@@ -673,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -685,8 +701,8 @@
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="33.28515625" customWidth="1"/>
-    <col min="5" max="5" width="50.5703125" customWidth="1"/>
-    <col min="6" max="6" width="57.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -701,7 +717,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -863,12 +879,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18.75">
+    <row r="34" spans="1:8" ht="18.75">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:8">
       <c r="B35" t="s">
         <v>23</v>
       </c>
@@ -879,8 +895,83 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="C40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="D41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="E42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="F43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="G44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="H45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="G46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="F47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="E48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="C50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
         <v>16</v>
       </c>
     </row>
@@ -892,10 +983,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -909,60 +1000,90 @@
     <col min="7" max="7" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75">
+    <row r="6" spans="1:4" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="18.75">
-      <c r="A13" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.75">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working basic Vis for numerics
</commit_message>
<xml_diff>
--- a/Java/API Builder/test/test.xlsx
+++ b/Java/API Builder/test/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <r>
       <rPr>
@@ -281,58 +281,40 @@
     <t>#Sets the amplitude of the analog measurement.</t>
   </si>
   <si>
-    <t>{how</t>
-  </si>
-  <si>
-    <t>{far</t>
-  </si>
-  <si>
-    <t>{down</t>
-  </si>
-  <si>
-    <t>{can</t>
-  </si>
-  <si>
-    <t>{this</t>
-  </si>
-  <si>
-    <t>{will</t>
-  </si>
-  <si>
-    <t>{go?}</t>
-  </si>
-  <si>
-    <t>My Vi</t>
-  </si>
-  <si>
-    <t>in:Test2:double</t>
-  </si>
-  <si>
     <t>""</t>
   </si>
   <si>
-    <t>MIT:TEST:TEST1 &lt;value&gt;</t>
-  </si>
-  <si>
-    <t>MIT:TEST:TEST2 &lt;value&gt;</t>
-  </si>
-  <si>
-    <t>Vi2</t>
-  </si>
-  <si>
-    <t>in:Test3:double</t>
-  </si>
-  <si>
-    <t>in:Test4:double</t>
-  </si>
-  <si>
-    <t>{utility</t>
-  </si>
-  <si>
-    <t>{lower}</t>
-  </si>
-  <si>
-    <t>in:Test1:integer</t>
+    <t>in:Frequency:double</t>
+  </si>
+  <si>
+    <t>Configure Mode</t>
+  </si>
+  <si>
+    <t>in:Operation:int</t>
+  </si>
+  <si>
+    <t>MIT:TEST:OPERATION &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>in:MakeOneUp:double</t>
+  </si>
+  <si>
+    <t># No command</t>
+  </si>
+  <si>
+    <t>{Subfolder</t>
+  </si>
+  <si>
+    <t>MIT:TEST:FREQ &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>Configure Write Something</t>
+  </si>
+  <si>
+    <t>in:Something:double</t>
+  </si>
+  <si>
+    <t>SOMETHING:IS:GOING:TO:HAPPEN: NOW</t>
   </si>
 </sst>
 </file>
@@ -689,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I35" sqref="I34:I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -879,12 +861,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="18.75">
+    <row r="34" spans="1:4" ht="18.75">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:4">
       <c r="B35" t="s">
         <v>23</v>
       </c>
@@ -895,83 +877,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="B39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="C40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="D41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="E42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="F43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="G44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="H45" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="G46" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="F47" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="E48" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="D49" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="C50" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="B51" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
         <v>16</v>
       </c>
     </row>
@@ -983,10 +890,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -994,95 +901,94 @@
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
     <col min="5" max="5" width="45" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.75">
+    <row r="6" spans="1:5" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="B7" t="s">
+    <row r="7" spans="1:5">
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="C7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="11" spans="1:5">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="B8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18.75">
+    <row r="13" spans="1:5" ht="18.75">
       <c r="A13" s="2"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
+      <c r="B13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Some code clean up
</commit_message>
<xml_diff>
--- a/Java/API Builder/test/test.xlsx
+++ b/Java/API Builder/test/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="18195" windowHeight="9015" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="18195" windowHeight="9015" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <r>
       <rPr>
@@ -284,9 +284,6 @@
     <t>""</t>
   </si>
   <si>
-    <t>in:Frequency:double</t>
-  </si>
-  <si>
     <t>Configure Mode</t>
   </si>
   <si>
@@ -314,7 +311,46 @@
     <t>in:Something:double</t>
   </si>
   <si>
-    <t>SOMETHING:IS:GOING:TO:HAPPEN: NOW</t>
+    <t>in:Test:string</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>out:Frequency:double</t>
+  </si>
+  <si>
+    <t>Bug Database for API Builder</t>
+  </si>
+  <si>
+    <t>Technology Field Parsing</t>
+  </si>
+  <si>
+    <t>Currently, LabVIEW PNP is hardcoded no matter what the user inputs into the technology field.</t>
+  </si>
+  <si>
+    <t>Rings and Booleans</t>
+  </si>
+  <si>
+    <t>No support currently for rings or booleans.</t>
+  </si>
+  <si>
+    <t>{Utility</t>
+  </si>
+  <si>
+    <t>Duplicate Template Vis</t>
+  </si>
+  <si>
+    <t>No check for the creation of duplicated template Vis -- although the API Builder doesn't create them</t>
+  </si>
+  <si>
+    <t>Configure Frequendacy</t>
+  </si>
+  <si>
+    <t>Arbitrary Column Size</t>
+  </si>
+  <si>
+    <t>Currently the user cannot write past 26 columns due to an arbitraily imposed limit.</t>
   </si>
 </sst>
 </file>
@@ -890,10 +926,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -934,13 +970,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
         <v>40</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -948,15 +984,15 @@
         <v>38</v>
       </c>
       <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
         <v>43</v>
-      </c>
-      <c r="E8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -964,31 +1000,57 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
         <v>47</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
         <v>48</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18.75">
-      <c r="A13" s="2"/>
-      <c r="B13" t="s">
+    <row r="14" spans="1:5" ht="18.75">
+      <c r="A14" s="2"/>
+      <c r="B14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>
@@ -999,12 +1061,56 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="90.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>